<commit_message>
Refactor, additional logs for errors
</commit_message>
<xml_diff>
--- a/test/second.xlsx
+++ b/test/second.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_CODE\python_code\ania\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863FA0A0-66AF-48CD-94E7-41158606884F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF36107-C856-475C-8811-207E503710DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-5595" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4350" yWindow="3135" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>A</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>9</t>
+  </si>
+  <si>
+    <t>gre</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -409,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,22 +479,20 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
+      <c r="A6" t="s">
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -496,21 +500,21 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -518,10 +522,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>16</v>
@@ -529,10 +533,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>16</v>
@@ -540,23 +544,34 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>